<commit_message>
add size variation that needs updated
</commit_message>
<xml_diff>
--- a/GHEDT/examples/GHE/BHE_size_variation.xlsx
+++ b/GHEDT/examples/GHE/BHE_size_variation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="GLHEPRO" sheetId="1" state="visible" r:id="rId2"/>
@@ -131,13 +131,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.48828125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.84"/>
@@ -158,90 +158,77 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>114.87</v>
+        <v>128.87</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>115.25</v>
+        <v>119.57</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>117.72</v>
+        <v>134.72</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>128.87</v>
+        <v>137.44</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>119.57</v>
+        <v>129.14</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>134.72</v>
+        <v>133.83</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>137.44</v>
+        <v>140.64</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>129.14</v>
+        <v>131.9</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>133.83</v>
+        <v>129.98</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>140.64</v>
+        <v>142.78</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>131.9</v>
+        <v>133.33</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>129.98</v>
+        <v>129.63</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>142.78</v>
+        <v>144.7</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>133.33</v>
+        <v>134.42</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>129.63</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>144.7</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>134.42</v>
-      </c>
-      <c r="D7" s="0" t="n">
         <v>129.55</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -258,13 +245,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="13.23"/>
@@ -286,85 +273,71 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>113.20894303</v>
+        <v>119.22529427</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>115.7072775</v>
+        <v>121.5288232</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>115.87716642</v>
+        <v>120.70378641</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>119.22529427</v>
+        <v>126.99645247</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>121.5288232</v>
+        <v>120.51610652</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>120.70378641</v>
+        <v>119.77592288</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>126.99645247</v>
+        <v>130.43706542</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>120.51610652</v>
+        <v>121.9395692</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>119.77592288</v>
+        <v>117.80425719</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>130.43706542</v>
+        <v>132.23783957</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>121.9395692</v>
+        <v>123.00573184</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>117.80425719</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>116.3731149</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>132.23783957</v>
+        <v>133.47347726</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>123.00573184</v>
+        <v>123.84726565</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>116.3731149</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>133.47347726</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>123.84726565</v>
-      </c>
-      <c r="D7" s="0" t="n">
         <v>116.1697562</v>
       </c>
     </row>
@@ -384,13 +357,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.23"/>
@@ -413,86 +386,72 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>113.20894303</v>
+        <v>120.7001</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>115.7072775</v>
+        <v>126.8004</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>115.87716642</v>
+        <v>136.6482</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>119.22529427</v>
+        <v>126.4279</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>121.5288232</v>
+        <v>121.129</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>120.70378641</v>
+        <v>123.3176</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>125.3595</v>
+        <v>130.1013</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>119.7787</v>
+        <v>122.078</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>123.4182</v>
+        <v>121.2471</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>128.8118</v>
+        <v>131.9653</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>121.3854</v>
+        <v>123.1104</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>121.3315</v>
+        <v>119.6726</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>131.4829</v>
+        <v>133.1795</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>122.2686</v>
+        <v>123.8189</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>119.8173</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>132.7208</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>122.8777</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>119.3368</v>
+        <v>119.2085</v>
       </c>
     </row>
   </sheetData>

</xml_diff>